<commit_message>
zaległy commit rankingu materiałów
</commit_message>
<xml_diff>
--- a/plan/Materiały budowlane - zestawienia.xlsx
+++ b/plan/Materiały budowlane - zestawienia.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="360" yWindow="60" windowWidth="11295" windowHeight="5580" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ranking" sheetId="1" r:id="rId1"/>
     <sheet name="Materiały budowlane - wady" sheetId="2" r:id="rId2"/>
     <sheet name="Termoizolacyjność" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="111">
   <si>
     <t>Bezpieczeństwo</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>Trwałość wg Glapy</t>
-  </si>
-  <si>
-    <t>Drewno</t>
   </si>
   <si>
     <t>Ceramika</t>
@@ -346,6 +343,72 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Zdrowie</t>
+  </si>
+  <si>
+    <t>Trwałość</t>
+  </si>
+  <si>
+    <t>Zawilgocenia</t>
+  </si>
+  <si>
+    <t>Szczelność</t>
+  </si>
+  <si>
+    <t>Termoizolacyjność</t>
+  </si>
+  <si>
+    <t>Koszt budowy</t>
+  </si>
+  <si>
+    <t>Łatwa obróbka</t>
+  </si>
+  <si>
+    <t>Ranking</t>
+  </si>
+  <si>
+    <t>Keramzybeton</t>
+  </si>
+  <si>
+    <t>usunięte/nie znaczące</t>
+  </si>
+  <si>
+    <t>Keramzytobeton</t>
+  </si>
+  <si>
+    <t>Termo Optiroc Akustyczny 18</t>
+  </si>
+  <si>
+    <t>1,7kWh</t>
+  </si>
+  <si>
+    <t>20min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beton  </t>
+  </si>
+  <si>
+    <t>4,25kWh</t>
+  </si>
+  <si>
+    <t>porotherm</t>
+  </si>
+  <si>
+    <t>6,7kWh</t>
+  </si>
+  <si>
+    <t>1h20min</t>
+  </si>
+  <si>
+    <t>12kWh</t>
+  </si>
+  <si>
+    <t>2h30min</t>
+  </si>
+  <si>
+    <t>50min</t>
   </si>
 </sst>
 </file>
@@ -670,7 +733,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -722,6 +785,7 @@
     <xf numFmtId="2" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1022,41 +1086,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="37.5703125" customWidth="1"/>
-    <col min="3" max="5" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="11" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>35</v>
-      </c>
       <c r="F1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="44" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -1069,12 +1136,12 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="30">
-      <c r="A3" s="43"/>
+    <row r="3" spans="1:8" ht="45">
+      <c r="A3" s="44"/>
       <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
@@ -1085,12 +1152,12 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="51" customHeight="1">
-      <c r="A4" s="43"/>
+      <c r="A4" s="44"/>
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
@@ -1103,14 +1170,14 @@
         <v>20</v>
       </c>
       <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="5" spans="1:8" ht="18.75">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="45" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -1127,14 +1194,14 @@
         <v>51</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="51" customHeight="1">
-      <c r="A6" s="44"/>
+      <c r="A6" s="45"/>
       <c r="B6" s="8" t="s">
         <v>8</v>
       </c>
@@ -1151,7 +1218,7 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="18.75">
-      <c r="A7" s="44"/>
+      <c r="A7" s="45"/>
       <c r="B7" s="8" t="s">
         <v>13</v>
       </c>
@@ -1166,14 +1233,14 @@
         <v>22</v>
       </c>
       <c r="F7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="8" spans="1:8" ht="51" customHeight="1">
-      <c r="A8" s="44"/>
+      <c r="A8" s="45"/>
       <c r="B8" s="8" t="s">
         <v>10</v>
       </c>
@@ -1187,7 +1254,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="51" customHeight="1">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="44" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -1202,11 +1269,11 @@
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="43"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="7" t="s">
         <v>9</v>
       </c>
@@ -1214,8 +1281,8 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:8" ht="18.75">
-      <c r="A11" s="44" t="s">
+    <row r="11" spans="1:8" ht="30">
+      <c r="A11" s="45" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -1232,14 +1299,14 @@
         <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="44"/>
+      <c r="A12" s="45"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
@@ -1253,7 +1320,7 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="44"/>
+      <c r="A13" s="45"/>
       <c r="B13" s="8" t="s">
         <v>15</v>
       </c>
@@ -1282,43 +1349,257 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="3" t="s">
+    <row r="18" spans="1:11">
+      <c r="F18" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="3"/>
+      <c r="B19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="43" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
+      <c r="D19" t="s">
+        <v>89</v>
+      </c>
+      <c r="E19" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" t="s">
+        <v>91</v>
+      </c>
+      <c r="G19" t="s">
+        <v>92</v>
+      </c>
+      <c r="H19" t="s">
+        <v>93</v>
+      </c>
+      <c r="I19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" t="s">
+        <v>94</v>
+      </c>
+      <c r="K19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <f t="shared" ref="B20:B24" si="1">D20*1+E20*2.55+F20*1.85+G20*1.1+H20*2+I20*0.75+J20*0.5+K20*0.25</f>
+        <v>51.35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20">
+        <v>9</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>8</v>
+      </c>
+      <c r="H20">
+        <v>8</v>
+      </c>
+      <c r="I20">
+        <v>10</v>
+      </c>
+      <c r="J20">
+        <v>10</v>
+      </c>
+      <c r="K20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="B21">
+        <f t="shared" si="1"/>
+        <v>56.05</v>
+      </c>
+      <c r="C21" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
+      <c r="D21">
+        <v>4.5</v>
+      </c>
+      <c r="E21">
+        <v>9</v>
+      </c>
+      <c r="G21">
+        <v>6</v>
+      </c>
+      <c r="H21">
+        <v>7</v>
+      </c>
+      <c r="I21">
+        <v>4</v>
+      </c>
+      <c r="J21">
+        <v>5</v>
+      </c>
+      <c r="K21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22">
+        <f>D22*1+E22*2.55+F22*1.85+G22*1.1+H22*2+I22*0.75+J22*0.5+K22*0.25</f>
+        <v>44.7</v>
+      </c>
+      <c r="D22">
+        <v>6.5</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>8</v>
+      </c>
+      <c r="H22">
+        <v>7</v>
+      </c>
+      <c r="I22">
+        <v>5</v>
+      </c>
+      <c r="J22">
+        <v>5</v>
+      </c>
+      <c r="K22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" t="s">
         <v>28</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B23">
+        <f t="shared" si="1"/>
+        <v>58.75</v>
+      </c>
+      <c r="D23">
+        <v>8.5</v>
+      </c>
+      <c r="E23">
+        <v>9</v>
+      </c>
+      <c r="G23">
+        <v>8</v>
+      </c>
+      <c r="H23">
+        <v>7</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>5</v>
+      </c>
+      <c r="K23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="1"/>
+        <v>71.25</v>
+      </c>
+      <c r="C24" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" t="s">
-        <v>33</v>
+      <c r="D24">
+        <v>7.5</v>
+      </c>
+      <c r="E24">
+        <v>10</v>
+      </c>
+      <c r="G24">
+        <v>10</v>
+      </c>
+      <c r="H24">
+        <v>10</v>
+      </c>
+      <c r="I24">
+        <v>7</v>
+      </c>
+      <c r="J24">
+        <v>2</v>
+      </c>
+      <c r="K24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="C30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" t="s">
+        <v>102</v>
+      </c>
+      <c r="G30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="C31" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F31" t="s">
+        <v>110</v>
+      </c>
+      <c r="G31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="C32" t="s">
+        <v>105</v>
+      </c>
+      <c r="E32" t="s">
+        <v>106</v>
+      </c>
+      <c r="F32" t="s">
+        <v>107</v>
+      </c>
+      <c r="G32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7">
+      <c r="C33" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" t="s">
+        <v>108</v>
+      </c>
+      <c r="F33" t="s">
+        <v>109</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1337,7 +1618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A5:D27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -1385,7 +1666,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1395,18 +1676,18 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s">
         <v>49</v>
-      </c>
-      <c r="B14" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
         <v>51</v>
-      </c>
-      <c r="B15" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="22" spans="2:4">
@@ -1447,8 +1728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1472,13 +1753,13 @@
   <sheetData>
     <row r="1" spans="2:23">
       <c r="B1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O1" s="36" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P1" s="36"/>
       <c r="Q1" s="37">
@@ -1487,60 +1768,60 @@
     </row>
     <row r="2" spans="2:23" ht="15.75" thickBot="1">
       <c r="H2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="2:23" ht="15.75" thickBot="1">
       <c r="B3" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O3" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="P3" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="P3" s="30" t="s">
+      <c r="Q3" s="31" t="s">
         <v>65</v>
-      </c>
-      <c r="Q3" s="31" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="4" spans="2:23" ht="15.75" thickBot="1">
       <c r="B4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E4" s="12">
         <v>0.247</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G4" s="12">
         <v>0.24</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I4" s="20">
         <f>IF(E4,E4,C4*G4)</f>
         <v>0.247</v>
       </c>
       <c r="K4" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L4" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M4" s="38"/>
       <c r="O4" s="32">
@@ -1557,23 +1838,23 @@
     </row>
     <row r="5" spans="2:23" ht="15.75" thickBot="1">
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" s="14">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G5" s="14">
         <v>0.21</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I5" s="20">
         <f>IF(E5,E5,C5*G5)</f>
@@ -1587,7 +1868,10 @@
         <f>G4+G5</f>
         <v>0.44999999999999996</v>
       </c>
-      <c r="M5" s="38"/>
+      <c r="M5" s="38">
+        <f>K5*L5</f>
+        <v>8.0999999999999989E-2</v>
+      </c>
       <c r="O5" s="26"/>
       <c r="P5" s="27"/>
       <c r="Q5" s="28">
@@ -1603,7 +1887,7 @@
     </row>
     <row r="7" spans="2:23" ht="15.75" thickBot="1">
       <c r="I7" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M7" s="39"/>
       <c r="O7" s="21"/>
@@ -1612,33 +1896,33 @@
     </row>
     <row r="8" spans="2:23" ht="15.75" thickBot="1">
       <c r="B8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="12">
         <v>0.31</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G8" s="12">
         <v>0.25</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I8" s="20">
         <f t="shared" ref="I8:I9" si="0">IF(E8,E8,C8*G8)</f>
         <v>0.31</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L8" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M8" s="38"/>
       <c r="O8" s="23">
@@ -1655,23 +1939,23 @@
     </row>
     <row r="9" spans="2:23" ht="15.75" thickBot="1">
       <c r="B9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" s="14">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G9" s="14">
         <v>0.2</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I9" s="20">
         <f t="shared" si="0"/>
@@ -1685,7 +1969,10 @@
         <f>G8+G9</f>
         <v>0.45</v>
       </c>
-      <c r="M9" s="38"/>
+      <c r="M9" s="38">
+        <f>K9*L9</f>
+        <v>8.5500000000000007E-2</v>
+      </c>
       <c r="O9" s="26"/>
       <c r="P9" s="27"/>
       <c r="Q9" s="28">
@@ -1701,7 +1988,7 @@
     </row>
     <row r="11" spans="2:23" ht="15.75" thickBot="1">
       <c r="I11" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M11" s="39"/>
       <c r="O11" s="21"/>
@@ -1710,33 +1997,33 @@
     </row>
     <row r="12" spans="2:23" ht="15.75" thickBot="1">
       <c r="B12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" s="12">
         <v>0.35</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G12" s="12">
         <v>0.38</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I12" s="20">
         <f t="shared" ref="I12:I13" si="1">IF(E12,E12,C12*G12)</f>
         <v>0.13299999999999998</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L12" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M12" s="38"/>
       <c r="O12" s="23">
@@ -1753,23 +2040,23 @@
     </row>
     <row r="13" spans="2:23" ht="15.75" thickBot="1">
       <c r="B13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E13" s="14">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G13" s="14">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I13" s="20">
         <f t="shared" si="1"/>
@@ -1783,7 +2070,10 @@
         <f>G12+G13</f>
         <v>0.45</v>
       </c>
-      <c r="M13" s="38"/>
+      <c r="M13" s="38">
+        <f>K13*L13</f>
+        <v>0.10350000000000001</v>
+      </c>
       <c r="O13" s="26"/>
       <c r="P13" s="27"/>
       <c r="Q13" s="28">
@@ -1799,37 +2089,37 @@
     </row>
     <row r="15" spans="2:23" ht="15.75" thickBot="1">
       <c r="B15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C15" s="12">
         <v>0.53</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G15" s="12">
         <v>0.25</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I15" s="20">
         <f>IF(E15,E15,C15*G15)</f>
         <v>0.13250000000000001</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L15" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M15" s="38"/>
       <c r="N15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O15" s="23">
         <f>100*100/(23.8*30)</f>
@@ -1846,23 +2136,23 @@
     </row>
     <row r="16" spans="2:23" ht="15.75" thickBot="1">
       <c r="B16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E16" s="14">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G16" s="14">
         <v>0.2</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I16" s="20">
         <f>IF(E16,E16,C16*G16)</f>
@@ -1876,9 +2166,12 @@
         <f>G15+G16</f>
         <v>0.45</v>
       </c>
-      <c r="M16" s="38"/>
+      <c r="M16" s="38">
+        <f>K16*L16</f>
+        <v>7.2000000000000008E-2</v>
+      </c>
       <c r="N16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O16" s="26"/>
       <c r="P16" s="27"/>
@@ -1887,10 +2180,10 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="2:19" ht="15.75" thickBot="1">
+    <row r="17" spans="2:20" ht="15.75" thickBot="1">
       <c r="M17" s="39"/>
       <c r="N17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O17" s="26"/>
       <c r="P17" s="27"/>
@@ -1898,58 +2191,63 @@
         <v>12</v>
       </c>
       <c r="R17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S17" s="21">
         <f>Q15+Q16+Q17</f>
         <v>159.72549019607843</v>
       </c>
-    </row>
-    <row r="18" spans="2:19" ht="15.75" thickBot="1">
+      <c r="T17" s="21">
+        <f>S17+55</f>
+        <v>214.72549019607843</v>
+      </c>
+    </row>
+    <row r="18" spans="2:20" ht="15.75" thickBot="1">
       <c r="B18" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I18" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M18" s="39"/>
       <c r="O18" s="21"/>
       <c r="P18" s="21"/>
       <c r="Q18" s="21"/>
-    </row>
-    <row r="19" spans="2:19" ht="15.75" thickBot="1">
+      <c r="T18" s="21"/>
+    </row>
+    <row r="19" spans="2:20" ht="15.75" thickBot="1">
       <c r="B19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E19" s="12">
         <v>0.16</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G19" s="12">
         <v>0.25</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I19" s="20">
         <f t="shared" ref="I19:I20" si="2">IF(E19,E19,C19*G19)</f>
         <v>0.16</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L19" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M19" s="38"/>
       <c r="N19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O19" s="23">
         <f>100*100/(19.9*59.9)</f>
@@ -1962,26 +2260,27 @@
         <f>P19*O19</f>
         <v>55.704230669205792</v>
       </c>
-    </row>
-    <row r="20" spans="2:19" ht="15.75" thickBot="1">
+      <c r="T19" s="21"/>
+    </row>
+    <row r="20" spans="2:20" ht="15.75" thickBot="1">
       <c r="B20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C20" s="14"/>
       <c r="D20" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E20" s="14">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G20" s="14">
         <v>0.2</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I20" s="20">
         <f t="shared" si="2"/>
@@ -1995,9 +2294,12 @@
         <f>G19+G20</f>
         <v>0.45</v>
       </c>
-      <c r="M20" s="38"/>
+      <c r="M20" s="38">
+        <f>K20*L20</f>
+        <v>7.6500000000000012E-2</v>
+      </c>
       <c r="N20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O20" s="26"/>
       <c r="P20" s="27"/>
@@ -2005,68 +2307,76 @@
         <f>$Q$1/(1/G20)</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="21" spans="2:19" ht="15.75" thickBot="1">
+      <c r="T20" s="21"/>
+    </row>
+    <row r="21" spans="2:20" ht="15.75" thickBot="1">
       <c r="M21" s="39"/>
       <c r="N21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O21" s="26"/>
       <c r="P21" s="27"/>
-      <c r="Q21" s="41"/>
+      <c r="Q21" s="41">
+        <v>12</v>
+      </c>
       <c r="R21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S21" s="21">
         <f>Q19+Q20+Q21</f>
-        <v>89.704230669205799</v>
-      </c>
-    </row>
-    <row r="22" spans="2:19" ht="15.75" thickBot="1">
+        <v>101.7042306692058</v>
+      </c>
+      <c r="T21" s="21">
+        <f t="shared" ref="T18:T28" si="3">S21+55</f>
+        <v>156.7042306692058</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" ht="15.75" thickBot="1">
       <c r="B22" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I22" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M22" s="39"/>
       <c r="O22" s="21"/>
       <c r="P22" s="21"/>
       <c r="Q22" s="21"/>
-    </row>
-    <row r="23" spans="2:19" ht="15.75" thickBot="1">
+      <c r="T22" s="21"/>
+    </row>
+    <row r="23" spans="2:20" ht="15.75" thickBot="1">
       <c r="B23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E23" s="12">
         <v>0.81</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G23" s="12">
         <v>0.18</v>
       </c>
       <c r="H23" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I23" s="20">
+        <f t="shared" ref="I23:I24" si="4">IF(E23,E23,C23*G23)</f>
+        <v>0.81</v>
+      </c>
+      <c r="K23" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="I23" s="20">
-        <f t="shared" ref="I23:I24" si="3">IF(E23,E23,C23*G23)</f>
-        <v>0.81</v>
-      </c>
-      <c r="K23" s="16" t="s">
-        <v>58</v>
-      </c>
       <c r="L23" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M23" s="38"/>
       <c r="N23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O23" s="23">
         <f>100*100/(19.9*33.3)</f>
@@ -2079,29 +2389,30 @@
         <f>P23*O23</f>
         <v>113.78212383237512</v>
       </c>
-    </row>
-    <row r="24" spans="2:19" ht="15.75" thickBot="1">
+      <c r="T23" s="21"/>
+    </row>
+    <row r="24" spans="2:20" ht="15.75" thickBot="1">
       <c r="B24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" s="14"/>
       <c r="D24" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E24" s="14">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G24" s="14">
         <v>0.27</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I24" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="K24" s="17">
@@ -2112,9 +2423,12 @@
         <f>G23+G24</f>
         <v>0.45</v>
       </c>
-      <c r="M24" s="38"/>
+      <c r="M24" s="38">
+        <f>K24*L24</f>
+        <v>7.2000000000000008E-2</v>
+      </c>
       <c r="N24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O24" s="26"/>
       <c r="P24" s="27"/>
@@ -2122,11 +2436,12 @@
         <f>$Q$1/(1/G24)</f>
         <v>45.900000000000006</v>
       </c>
-    </row>
-    <row r="25" spans="2:19" ht="15.75" thickBot="1">
+      <c r="T24" s="21"/>
+    </row>
+    <row r="25" spans="2:20" ht="15.75" thickBot="1">
       <c r="M25" s="39"/>
       <c r="N25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O25" s="26"/>
       <c r="P25" s="27"/>
@@ -2134,27 +2449,118 @@
         <v>7.5</v>
       </c>
       <c r="R25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S25" s="21">
         <f>Q23+Q24+Q25</f>
         <v>167.18212383237511</v>
       </c>
+      <c r="T25" s="21">
+        <f t="shared" si="3"/>
+        <v>222.18212383237511</v>
+      </c>
+    </row>
+    <row r="26" spans="2:20">
+      <c r="T26" s="21"/>
+    </row>
+    <row r="27" spans="2:20" ht="15.75" thickBot="1">
+      <c r="B27" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="I27" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="T27" s="21"/>
+    </row>
+    <row r="28" spans="2:20" ht="15.75" thickBot="1">
+      <c r="B28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="12">
+        <v>0.73</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G28" s="12">
+        <v>0.18</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I28" s="20">
+        <f t="shared" ref="I28:I29" si="5">IF(E28,E28,C28*G28)</f>
+        <v>0.73</v>
+      </c>
+      <c r="K28" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="L28" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="S28">
+        <v>200</v>
+      </c>
+      <c r="T28" s="21">
+        <f>S28+35</f>
+        <v>235</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20" ht="15.75" thickBot="1">
+      <c r="B29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E29" s="14">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G29" s="14">
+        <v>0.27</v>
+      </c>
+      <c r="H29" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I29" s="20">
+        <f t="shared" si="5"/>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="K29" s="17">
+        <f>ROUND(1/((G28/I28)+(G29/I29)),2)</f>
+        <v>0.16</v>
+      </c>
+      <c r="L29" s="19">
+        <f>G28+G29</f>
+        <v>0.45</v>
+      </c>
+      <c r="M29" s="38">
+        <f>K29*L29</f>
+        <v>7.2000000000000008E-2</v>
+      </c>
     </row>
     <row r="37" spans="1:7">
       <c r="B37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C37" s="34">
         <v>170</v>
       </c>
       <c r="F37" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B38">
         <v>5</v>
@@ -2164,7 +2570,7 @@
         <v>20</v>
       </c>
       <c r="D38" s="35">
-        <f t="shared" ref="D38:D41" si="4">$C$37/C38</f>
+        <f t="shared" ref="D38:D41" si="6">$C$37/C38</f>
         <v>8.5</v>
       </c>
     </row>
@@ -2173,15 +2579,15 @@
         <v>10</v>
       </c>
       <c r="C39">
-        <f t="shared" ref="C39:C42" si="5">1/B39*100</f>
+        <f t="shared" ref="C39:C42" si="7">1/B39*100</f>
         <v>10</v>
       </c>
       <c r="D39" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="F39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G39">
         <v>0.31</v>
@@ -2192,15 +2598,15 @@
         <v>12</v>
       </c>
       <c r="C40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8.3333333333333321</v>
       </c>
       <c r="D40" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>20.400000000000002</v>
       </c>
       <c r="F40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G40">
         <v>0.25</v>
@@ -2211,15 +2617,15 @@
         <v>15</v>
       </c>
       <c r="C41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6.666666666666667</v>
       </c>
       <c r="D41" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>25.5</v>
       </c>
       <c r="F41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G41">
         <f>G39/G40</f>
@@ -2231,7 +2637,7 @@
         <v>20</v>
       </c>
       <c r="C42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="D42" s="35">
@@ -2241,12 +2647,12 @@
     </row>
     <row r="43" spans="1:7">
       <c r="C43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="D45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -2263,7 +2669,7 @@
         <v>10</v>
       </c>
       <c r="E47">
-        <f t="shared" ref="E47:E49" si="6">$C$37/(1/D47*100)</f>
+        <f t="shared" ref="E47:E49" si="8">$C$37/(1/D47*100)</f>
         <v>17</v>
       </c>
     </row>
@@ -2272,7 +2678,7 @@
         <v>15</v>
       </c>
       <c r="E48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>25.5</v>
       </c>
     </row>
@@ -2281,7 +2687,7 @@
         <v>20</v>
       </c>
       <c r="E49">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>34</v>
       </c>
     </row>

</xml_diff>